<commit_message>
Adding treatments and data for Guadeloupe
</commit_message>
<xml_diff>
--- a/Prototypes/Gliricidia/GuadeloupeData.xlsx
+++ b/Prototypes/Gliricidia/GuadeloupeData.xlsx
@@ -3930,7 +3930,7 @@
   <dimension ref="A3:Q57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5256,11 +5256,11 @@
         <v>35184.124463519314</v>
       </c>
       <c r="C47">
-        <f>O9*$E$5*1000</f>
+        <f t="shared" ref="C47:C56" si="12">O9*$E$5*1000</f>
         <v>53.091847192281655</v>
       </c>
       <c r="D47">
-        <f>Q9*$E$5*1000</f>
+        <f t="shared" ref="D47:D56" si="13">Q9*$E$5*1000</f>
         <v>0</v>
       </c>
       <c r="E47">
@@ -5277,11 +5277,11 @@
         <v>35236.038626609443</v>
       </c>
       <c r="C48">
-        <f>O10*$E$5*1000</f>
+        <f t="shared" si="12"/>
         <v>385.9808460260781</v>
       </c>
       <c r="D48">
-        <f>Q10*$E$5*1000</f>
+        <f t="shared" si="13"/>
         <v>403.49344978165851</v>
       </c>
       <c r="E48">
@@ -5298,11 +5298,11 @@
         <v>35236.038626609443</v>
       </c>
       <c r="C49">
-        <f>O11*$E$5*1000</f>
+        <f t="shared" si="12"/>
         <v>182.34088419267016</v>
       </c>
       <c r="D49">
-        <f>Q11*$E$5*1000</f>
+        <f t="shared" si="13"/>
         <v>146.7248908296927</v>
       </c>
     </row>
@@ -5315,11 +5315,11 @@
         <v>35290.836909871243</v>
       </c>
       <c r="C50">
-        <f>O12*$E$5*1000</f>
+        <f t="shared" si="12"/>
         <v>362.55186062126631</v>
       </c>
       <c r="D50">
-        <f>Q12*$E$5*1000</f>
+        <f t="shared" si="13"/>
         <v>696.94323144104601</v>
       </c>
       <c r="E50">
@@ -5336,11 +5336,11 @@
         <v>35290.836909871243</v>
       </c>
       <c r="C51">
-        <f>O13*$E$5*1000</f>
+        <f t="shared" si="12"/>
         <v>171.74329434215599</v>
       </c>
       <c r="D51">
-        <f>Q13*$E$5*1000</f>
+        <f t="shared" si="13"/>
         <v>293.44978165938539</v>
       </c>
     </row>
@@ -5353,11 +5353,11 @@
         <v>35348.519313304721</v>
       </c>
       <c r="C52">
-        <f>O14*$E$5*1000</f>
+        <f t="shared" si="12"/>
         <v>237.56263914902607</v>
       </c>
       <c r="D52">
-        <f>Q14*$E$5*1000</f>
+        <f t="shared" si="13"/>
         <v>696.94323144104601</v>
       </c>
       <c r="E52">
@@ -5374,11 +5374,11 @@
         <v>35348.519313304721</v>
       </c>
       <c r="C53">
-        <f>O15*$E$5*1000</f>
+        <f t="shared" si="12"/>
         <v>46.650174930204713</v>
       </c>
       <c r="D53">
-        <f>Q15*$E$5*1000</f>
+        <f t="shared" si="13"/>
         <v>146.7248908296927</v>
       </c>
     </row>
@@ -5391,11 +5391,11 @@
         <v>35400.43347639485</v>
       </c>
       <c r="C54">
-        <f>O16*$E$5*1000</f>
+        <f t="shared" si="12"/>
         <v>226.75725341909006</v>
       </c>
       <c r="D54">
-        <f>Q16*$E$5*1000</f>
+        <f t="shared" si="13"/>
         <v>880.34934497816437</v>
       </c>
       <c r="E54">
@@ -5412,11 +5412,11 @@
         <v>35400.43347639485</v>
       </c>
       <c r="C55">
-        <f>O17*$E$5*1000</f>
+        <f t="shared" si="12"/>
         <v>86.754779658621047</v>
       </c>
       <c r="D55">
-        <f>Q17*$E$5*1000</f>
+        <f t="shared" si="13"/>
         <v>330.13100436680901</v>
       </c>
     </row>
@@ -5429,11 +5429,11 @@
         <v>35461</v>
       </c>
       <c r="C56">
-        <f>O18*$E$5*1000</f>
+        <f t="shared" si="12"/>
         <v>101.76803194684915</v>
       </c>
       <c r="D56">
-        <f>Q18*$E$5*1000</f>
+        <f t="shared" si="13"/>
         <v>146.7248908296927</v>
       </c>
       <c r="E56">

</xml_diff>

<commit_message>
Started fitting to dataset
</commit_message>
<xml_diff>
--- a/Prototypes/Gliricidia/GuadeloupeData.xlsx
+++ b/Prototypes/Gliricidia/GuadeloupeData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="20">
   <si>
     <t>12 month</t>
   </si>
@@ -82,6 +82,9 @@
   <si>
     <t>GuadeloupeHarvest02Month</t>
   </si>
+  <si>
+    <t>Gliricidia.AboveGround.Wt</t>
+  </si>
 </sst>
 </file>
 
@@ -116,11 +119,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -269,7 +273,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$34:$C$39</c:f>
+              <c:f>Sheet1!$D$34:$D$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -357,7 +361,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$34:$D$39</c:f>
+              <c:f>Sheet1!$E$34:$E$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -445,7 +449,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$34:$E$39</c:f>
+              <c:f>Sheet1!$F$34:$F$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -822,7 +826,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$40:$C$46</c:f>
+              <c:f>Sheet1!$D$40:$D$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -916,7 +920,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$40:$D$46</c:f>
+              <c:f>Sheet1!$E$40:$E$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1010,7 +1014,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$40:$E$46</c:f>
+              <c:f>Sheet1!$F$40:$F$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1396,7 +1400,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$47:$C$56</c:f>
+              <c:f>Sheet1!$D$47:$D$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1508,7 +1512,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$47:$D$56</c:f>
+              <c:f>Sheet1!$E$47:$E$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1620,7 +1624,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$47:$E$56</c:f>
+              <c:f>Sheet1!$F$47:$F$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1863,6 +1867,962 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$S$33</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gliricidia.Leaf.Live.Wt</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$R$34:$R$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>382.14438342985062</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1751.4978428322415</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4171.4279338543429</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5409.7355298586226</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7011.6153356947761</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4909.3007278020277</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>272.12268646760583</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1466.848726400782</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3619.9403497752191</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$S$34:$S$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>272.10071530758057</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>871.14849785407705</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1457.0174535050062</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>971.30758226037051</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>812.48869814020009</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>287.46666666666687</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>195.6612399643173</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>752.15655664585154</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1282.9170383586077</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1DB3-40C3-9ED7-EE5631C8FEA6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$T$33</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gliricidia.Stem.Live.Wt</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.44461570428696412"/>
+                  <c:y val="1.8101851851851852E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$R$34:$R$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>382.14438342985062</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1751.4978428322415</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4171.4279338543429</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5409.7355298586226</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7011.6153356947761</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4909.3007278020277</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>272.12268646760583</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1466.848726400782</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3619.9403497752191</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$T$34:$T$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>110.04366812227003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>880.34934497816437</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2714.4104803493365</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4438.4279475982521</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6199.1266375545765</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4621.8340611353606</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>76.461446503288556</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>714.69216975493043</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2337.0233114166117</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1DB3-40C3-9ED7-EE5631C8FEA6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="487945392"/>
+        <c:axId val="487947688"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="487945392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="487947688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="487947688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="487945392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$S$33</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gliricidia.Leaf.Live.Wt</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Sheet1!$R$34:$R$36,Sheet1!$R$40:$R$42)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>382.14438342985062</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1751.4978428322415</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4171.4279338543429</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>272.12268646760583</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1466.848726400782</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3619.9403497752191</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Sheet1!$S$34:$S$36,Sheet1!$S$40:$S$42)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>272.10071530758057</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>871.14849785407705</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1457.0174535050062</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>195.6612399643173</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>752.15655664585154</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1282.9170383586077</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5649-4687-99DC-18168C9E0845}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="486233032"/>
+        <c:axId val="486232376"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="486233032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="486232376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="486232376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="486233032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1983,6 +2943,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3531,17 +4571,1049 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>13335</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>956310</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>13335</xdr:rowOff>
@@ -3565,13 +5637,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>171450</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>53340</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>937260</xdr:colOff>
       <xdr:row>63</xdr:row>
       <xdr:rowOff>53340</xdr:rowOff>
@@ -3597,13 +5669,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>167640</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3622,6 +5694,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>135255</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>135255</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1748790</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>59055</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>59055</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3927,191 +6059,196 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:Q57"/>
+  <dimension ref="A3:T57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="M33" workbookViewId="0">
+      <selection activeCell="R40" activeCellId="1" sqref="R33:S36 R40:S42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="23.7890625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.15625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7890625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5234375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.26171875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.15625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.734375" customWidth="1"/>
-    <col min="10" max="11" width="24.578125" customWidth="1"/>
-    <col min="12" max="12" width="24.578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="11.68359375" customWidth="1"/>
-    <col min="15" max="15" width="11.68359375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.15625" customWidth="1"/>
+    <col min="4" max="4" width="17.7890625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5234375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.26171875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.15625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.734375" customWidth="1"/>
+    <col min="11" max="12" width="24.578125" customWidth="1"/>
+    <col min="13" max="13" width="24.578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="11.68359375" customWidth="1"/>
+    <col min="16" max="16" width="23.7890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="1">
         <v>35461</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1"/>
+      <c r="D3">
         <f>B3-B4</f>
         <v>336</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>0.7</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="1">
         <v>35125</v>
       </c>
-      <c r="E4">
+      <c r="C4" s="1"/>
+      <c r="F4">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="E5">
-        <f>E3*E4</f>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="F5">
+        <f>F3*F4</f>
         <v>2.0999999999999996</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="C7" t="s">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="D7" t="s">
         <v>0</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>3</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="D8" t="s">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="E8" t="s">
         <v>5</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>6</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>8</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>5</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="2">
-        <f>(DATE(1996,3,1)+C9)</f>
+        <f>(DATE(1996,3,1)+D9)</f>
         <v>35184.124463519314</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2"/>
+      <c r="D9">
         <v>59.124463519313302</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>0.129571769194086</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>5.2401746724890501E-2</v>
       </c>
-      <c r="G9" s="2">
-        <f>(DATE(1996,3,1)+H9)</f>
+      <c r="H9" s="2">
+        <f>(DATE(1996,3,1)+I9)</f>
         <v>35183.372881355936</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>58.372881355932201</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>9.3172019030627301E-2</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>3.64102126206136E-2</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>4</v>
       </c>
-      <c r="M9" s="2">
-        <f>(DATE(1996,3,1)+N9)</f>
+      <c r="N9" s="2">
+        <f>(DATE(1996,3,1)+O9)</f>
         <v>35182.624765876244</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>57.624765876241298</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>2.52818319963246E-2</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>58.621276595744597</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="2">
-        <f t="shared" ref="B10:B26" si="0">(DATE(1996,3,1)+C10)</f>
+        <f t="shared" ref="B10:B26" si="0">(DATE(1996,3,1)+D10)</f>
         <v>35236.038626609443</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2"/>
+      <c r="D10">
         <v>111.03862660944201</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>0.414832618025751</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>0.41921397379912601</v>
       </c>
-      <c r="G10" s="2">
-        <f t="shared" ref="G10:G26" si="1">(DATE(1996,3,1)+H10)</f>
+      <c r="H10" s="2">
+        <f t="shared" ref="H10:H26" si="1">(DATE(1996,3,1)+I10)</f>
         <v>35236.050847457627</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>111.050847457627</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>0.35816978887897699</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>0.34032960464520501</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>4</v>
       </c>
-      <c r="M10" s="2">
-        <f t="shared" ref="M10:M30" si="2">(DATE(1996,3,1)+N10)</f>
+      <c r="N10" s="2">
+        <f t="shared" ref="N10:N30" si="2">(DATE(1996,3,1)+O10)</f>
         <v>35234.894335088524</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>109.894335088525</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>0.18380040286956101</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>112.953191489361</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>0.19213973799126599</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -4119,49 +6256,50 @@
         <f t="shared" si="0"/>
         <v>35290.836909871243</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2"/>
+      <c r="D11">
         <v>165.83690987124399</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>0.69381783500238403</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>1.2925764192139699</v>
       </c>
-      <c r="G11" s="2">
+      <c r="H11" s="2">
         <f t="shared" si="1"/>
         <v>35290.152542372882</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>165.15254237288099</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>0.61091287540886097</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>1.1128682435317201</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>4</v>
       </c>
-      <c r="M11" s="2">
+      <c r="N11" s="2">
         <f t="shared" si="2"/>
         <v>35234.7993426865</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>109.799342686503</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>8.6828992472700095E-2</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>112.953191489361</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>6.9868995633187006E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -4169,49 +6307,50 @@
         <f t="shared" si="0"/>
         <v>35348.519313304721</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2"/>
+      <c r="D12">
         <v>223.51931330472101</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>0.46252742012398601</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>2.1135371179039302</v>
       </c>
-      <c r="G12" s="2">
+      <c r="H12" s="2">
         <f t="shared" si="1"/>
         <v>35348.52542372881</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>223.525423728813</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>0.21899717514124201</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>0.128357954060284</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>4</v>
       </c>
-      <c r="M12" s="2">
+      <c r="N12" s="2">
         <f t="shared" si="2"/>
         <v>35288.369120401454</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>163.369120401456</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>0.172643743152984</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>165.85531914893599</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>0.33187772925764097</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -4219,49 +6358,50 @@
         <f t="shared" si="0"/>
         <v>35400.43347639485</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2"/>
+      <c r="D13">
         <v>275.43347639484898</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>0.386899380066762</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>2.9519650655021801</v>
       </c>
-      <c r="G13" s="2">
+      <c r="H13" s="2">
         <f t="shared" si="1"/>
         <v>35401.203389830509</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>276.203389830508</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>0.256801962533452</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>0.39873623089403099</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>4</v>
       </c>
-      <c r="M13" s="2">
+      <c r="N13" s="2">
         <f t="shared" si="2"/>
         <v>35291.022970632926</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>166.022970632929</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <v>8.1782521115312395E-2</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <v>165.85531914893599</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>0.13973799126637401</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -4269,49 +6409,50 @@
         <f t="shared" si="0"/>
         <v>35461</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2"/>
+      <c r="D14">
         <v>336</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>0.136888888888889</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>2.2008733624454102</v>
       </c>
-      <c r="G14" s="2">
+      <c r="H14" s="2">
         <f t="shared" si="1"/>
         <v>35462.423728813555</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>337.42372881355902</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>0.110552334225393</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>0.56903765690376495</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>4</v>
       </c>
-      <c r="M14" s="2">
+      <c r="N14" s="2">
         <f t="shared" si="2"/>
         <v>35348.653673534296</v>
       </c>
-      <c r="N14">
+      <c r="O14">
         <v>223.65367353429599</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <v>0.113125066261441</v>
       </c>
-      <c r="P14">
+      <c r="Q14">
         <v>224.47659574468</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <v>0.33187772925764097</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -4319,43 +6460,44 @@
         <f t="shared" si="0"/>
         <v>35182.682403433479</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="2"/>
+      <c r="D15">
         <v>57.682403433476402</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>0</v>
       </c>
-      <c r="G15" s="2">
+      <c r="H15" s="2">
         <f t="shared" si="1"/>
         <v>35183.372881355936</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>58.372881355932201</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>0</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>4</v>
       </c>
-      <c r="M15" s="2">
+      <c r="N15" s="2">
         <f t="shared" si="2"/>
         <v>35348.564618157397</v>
       </c>
-      <c r="N15">
+      <c r="O15">
         <v>223.56461815740099</v>
       </c>
-      <c r="O15">
+      <c r="P15">
         <v>2.2214369014383201E-2</v>
       </c>
-      <c r="P15">
+      <c r="Q15">
         <v>224.47659574468</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
         <v>6.9868995633187006E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -4363,43 +6505,44 @@
         <f t="shared" si="0"/>
         <v>35236.038626609443</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="2"/>
+      <c r="D16">
         <v>111.03862660944201</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>2.2832618025751199E-2</v>
       </c>
-      <c r="G16" s="2">
+      <c r="H16" s="2">
         <f t="shared" si="1"/>
         <v>35236.050847457627</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>111.050847457627</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>1.4310139756169999E-2</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>4</v>
       </c>
-      <c r="M16" s="2">
+      <c r="N16" s="2">
         <f t="shared" si="2"/>
         <v>35399.391490263988</v>
       </c>
-      <c r="N16">
+      <c r="O16">
         <v>274.39149026398502</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <v>0.107979644485281</v>
       </c>
-      <c r="P16">
+      <c r="Q16">
         <v>275.94893617021199</v>
       </c>
-      <c r="Q16">
+      <c r="R16">
         <v>0.41921397379912601</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -4407,43 +6550,44 @@
         <f t="shared" si="0"/>
         <v>35289.394849785407</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="2"/>
+      <c r="D17">
         <v>164.39484978540699</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>0.15873342870767701</v>
       </c>
-      <c r="G17" s="2">
+      <c r="H17" s="2">
         <f t="shared" si="1"/>
         <v>35290.152542372882</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>165.15254237288099</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>0.13810585786500101</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>4</v>
       </c>
-      <c r="M17" s="2">
+      <c r="N17" s="2">
         <f t="shared" si="2"/>
         <v>35399.326182987592</v>
       </c>
-      <c r="N17">
+      <c r="O17">
         <v>274.32618298759502</v>
       </c>
-      <c r="O17">
+      <c r="P17">
         <v>4.1311799837438601E-2</v>
       </c>
-      <c r="P17">
+      <c r="Q17">
         <v>277.37872340425503</v>
       </c>
-      <c r="Q17">
+      <c r="R17">
         <v>0.157205240174671</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -4451,43 +6595,44 @@
         <f t="shared" si="0"/>
         <v>35348.519313304721</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2"/>
+      <c r="D18">
         <v>223.51931330472101</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>0.23852742012398601</v>
       </c>
-      <c r="G18" s="2">
+      <c r="H18" s="2">
         <f t="shared" si="1"/>
         <v>35348.52542372881</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>223.525423728813</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>1.02252453166813E-2</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>4</v>
       </c>
-      <c r="M18" s="2">
+      <c r="N18" s="2">
         <f t="shared" si="2"/>
         <v>35459.676043396823</v>
       </c>
-      <c r="N18">
+      <c r="O18">
         <v>334.676043396826</v>
       </c>
-      <c r="O18">
+      <c r="P18">
         <v>4.8460967593737699E-2</v>
       </c>
-      <c r="P18">
+      <c r="Q18">
         <v>336</v>
       </c>
-      <c r="Q18">
+      <c r="R18">
         <v>6.9868995633187006E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -4495,37 +6640,38 @@
         <f t="shared" si="0"/>
         <v>35400.43347639485</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="2"/>
+      <c r="D19">
         <v>275.43347639484898</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>0.13801049117787301</v>
       </c>
-      <c r="G19" s="2">
+      <c r="H19" s="2">
         <f t="shared" si="1"/>
         <v>35401.203389830509</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>276.203389830508</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>9.1012488849241596E-2</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>1</v>
       </c>
-      <c r="M19" s="2">
+      <c r="N19" s="2">
         <f t="shared" si="2"/>
         <v>35182.595080750609</v>
       </c>
-      <c r="N19">
+      <c r="O19">
         <v>57.595080750609597</v>
       </c>
-      <c r="O19">
+      <c r="P19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -4533,37 +6679,38 @@
         <f t="shared" si="0"/>
         <v>35461</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2"/>
+      <c r="D20">
         <v>336</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>8.7111111111111098E-2</v>
       </c>
-      <c r="G20" s="2">
+      <c r="H20" s="2">
         <f t="shared" si="1"/>
         <v>35461</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>336</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>0.14122807017543801</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>1</v>
       </c>
-      <c r="M20" s="2">
+      <c r="N20" s="2">
         <f t="shared" si="2"/>
         <v>35234.728098384985</v>
       </c>
-      <c r="N20">
+      <c r="O20">
         <v>109.72809838498701</v>
       </c>
-      <c r="O20">
+      <c r="P20">
         <v>1.4100434675053701E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -4571,43 +6718,44 @@
         <f t="shared" si="0"/>
         <v>35184.124463519314</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="2"/>
+      <c r="D21">
         <v>59.124463519313302</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>0.129571769194086</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>6.9868995633187006E-2</v>
       </c>
-      <c r="G21" s="2">
+      <c r="H21" s="2">
         <f t="shared" si="1"/>
         <v>35183.372881355936</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>58.372881355932201</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>9.3172019030627301E-2</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>1.9673810946972702E-2</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>1</v>
       </c>
-      <c r="M21" s="2">
+      <c r="N21" s="2">
         <f t="shared" si="2"/>
         <v>35290.993285507298</v>
       </c>
-      <c r="N21">
+      <c r="O21">
         <v>165.993285507297</v>
       </c>
-      <c r="O21">
+      <c r="P21">
         <v>5.1478955366293301E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -4615,43 +6763,44 @@
         <f t="shared" si="0"/>
         <v>35236.038626609443</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="2"/>
+      <c r="D22">
         <v>111.03862660944201</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>0.44594372913686198</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>0.43668122270742299</v>
       </c>
-      <c r="G22" s="2">
+      <c r="H22" s="2">
         <f t="shared" si="1"/>
         <v>35236.050847457627</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>111.050847457627</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>0.376590841510555</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>0.34032960464520501</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
         <v>1</v>
       </c>
-      <c r="M22" s="2">
+      <c r="N22" s="2">
         <f t="shared" si="2"/>
         <v>35348.582429232782</v>
       </c>
-      <c r="N22">
+      <c r="O22">
         <v>223.58242923277999</v>
       </c>
-      <c r="O22">
+      <c r="P22">
         <v>4.0396508463794702E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -4659,43 +6808,44 @@
         <f t="shared" si="0"/>
         <v>35289.394849785407</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="2"/>
+      <c r="D23">
         <v>164.39484978540699</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>0.88673342870767702</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>1.31004366812227</v>
       </c>
-      <c r="G23" s="2">
+      <c r="H23" s="2">
         <f t="shared" si="1"/>
         <v>35290.152542372882</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>165.15254237288099</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>0.76442164733868501</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <v>1.12953633336179</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
         <v>1</v>
       </c>
-      <c r="M23" s="2">
+      <c r="N23" s="2">
         <f t="shared" si="2"/>
         <v>35400.68576174153</v>
       </c>
-      <c r="N23">
+      <c r="O23">
         <v>275.68576174152702</v>
       </c>
-      <c r="O23">
+      <c r="P23">
         <v>2.9215111142524001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -4703,43 +6853,44 @@
         <f t="shared" si="0"/>
         <v>35349.961373390557</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="2"/>
+      <c r="D24">
         <v>224.96137339055699</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>0.88561182641869296</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>2.1484716157205201</v>
       </c>
-      <c r="G24" s="2">
+      <c r="H24" s="2">
         <f t="shared" si="1"/>
         <v>35349.949152542373</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>224.94915254237199</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>0.99884775498067102</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>1.26636495602425</v>
       </c>
-      <c r="L24" t="s">
+      <c r="M24" t="s">
         <v>1</v>
       </c>
-      <c r="M24" s="2">
+      <c r="N24" s="2">
         <f t="shared" si="2"/>
         <v>35459.687917447081</v>
       </c>
-      <c r="N24">
+      <c r="O24">
         <v>334.68791744707897</v>
       </c>
-      <c r="O24">
+      <c r="P24">
         <v>6.0582393893345403E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -4747,49 +6898,50 @@
         <f t="shared" si="0"/>
         <v>35400.43347639485</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="2"/>
+      <c r="D25">
         <v>275.43347639484898</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>1.0588993800667601</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>3.4410480349344899</v>
       </c>
-      <c r="G25" s="2">
+      <c r="H25" s="2">
         <f t="shared" si="1"/>
         <v>35399.779661016946</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>274.77966101694898</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>1.1532671721676999</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <v>1.53674323285799</v>
       </c>
-      <c r="L25" t="s">
+      <c r="M25" t="s">
         <v>2</v>
       </c>
-      <c r="M25" s="2">
+      <c r="N25" s="2">
         <f t="shared" si="2"/>
         <v>35182.660388026998</v>
       </c>
-      <c r="N25">
+      <c r="O25">
         <v>57.6603880269993</v>
       </c>
-      <c r="O25">
+      <c r="P25">
         <v>6.16461108951478E-2</v>
       </c>
-      <c r="P25">
+      <c r="Q25">
         <v>60.051063829787203</v>
       </c>
-      <c r="Q25">
+      <c r="R25">
         <v>1.7467248908296502E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -4797,133 +6949,134 @@
         <f t="shared" si="0"/>
         <v>35462.442060085836</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="2"/>
+      <c r="D26">
         <v>337.442060085837</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>1.0639732951835901</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>3.4235807860262</v>
       </c>
-      <c r="G26" s="2">
+      <c r="H26" s="2">
         <f t="shared" si="1"/>
         <v>35462.423728813555</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <v>337.42372881355902</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <v>1.2894997026464401</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <v>2.3264281444795398</v>
       </c>
-      <c r="L26" t="s">
+      <c r="M26" t="s">
         <v>2</v>
       </c>
-      <c r="M26" s="2">
+      <c r="N26" s="2">
         <f t="shared" si="2"/>
         <v>35236.313284093718</v>
       </c>
-      <c r="N26">
+      <c r="O26">
         <v>111.31328409372</v>
       </c>
-      <c r="O26">
+      <c r="P26">
         <v>0.23231084567268601</v>
       </c>
-      <c r="P26">
+      <c r="Q26">
         <v>128.68085106382901</v>
       </c>
-      <c r="Q26">
+      <c r="R26">
         <v>0.19213973799126599</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="L27" t="s">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="M27" t="s">
         <v>2</v>
       </c>
-      <c r="M27" s="2">
+      <c r="N27" s="2">
         <f t="shared" si="2"/>
         <v>35291.302010813866</v>
       </c>
-      <c r="N27">
+      <c r="O27">
         <v>166.30201081386701</v>
       </c>
-      <c r="O27">
+      <c r="P27">
         <v>0.366636039156094</v>
       </c>
-      <c r="P27">
+      <c r="Q27">
         <v>165.85531914893599</v>
       </c>
-      <c r="Q27">
+      <c r="R27">
         <v>0.45414847161571897</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="L28" t="s">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="M28" t="s">
         <v>2</v>
       </c>
-      <c r="M28" s="2">
+      <c r="N28" s="2">
         <f t="shared" si="2"/>
         <v>35350.35166272043</v>
       </c>
-      <c r="N28">
+      <c r="O28">
         <v>225.351662720429</v>
       </c>
-      <c r="O28">
+      <c r="P28">
         <v>0.44648902710534699</v>
       </c>
-      <c r="P28">
+      <c r="Q28">
         <v>224.47659574468</v>
       </c>
-      <c r="Q28">
+      <c r="R28">
         <v>0.62882096069868898</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="L29" t="s">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="M29" t="s">
         <v>2</v>
       </c>
-      <c r="M29" s="2">
+      <c r="N29" s="2">
         <f t="shared" si="2"/>
         <v>35401.190408877264</v>
       </c>
-      <c r="N29">
+      <c r="O29">
         <v>276.19040887726601</v>
       </c>
-      <c r="O29">
+      <c r="P29">
         <v>0.54437572887585195</v>
       </c>
-      <c r="P29">
+      <c r="Q29">
         <v>277.37872340425503</v>
       </c>
-      <c r="Q29">
+      <c r="R29">
         <v>0.96069868995633101</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="L30" t="s">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="M30" t="s">
         <v>2</v>
       </c>
-      <c r="M30" s="2">
+      <c r="N30" s="2">
         <f t="shared" si="2"/>
         <v>35460.228186733577</v>
       </c>
-      <c r="N30">
+      <c r="O30">
         <v>335.22818673357602</v>
       </c>
-      <c r="O30">
+      <c r="P30">
         <v>0.61210729052549695</v>
       </c>
-      <c r="P30">
+      <c r="Q30">
         <v>337.42978723404201</v>
       </c>
-      <c r="Q30">
+      <c r="R30">
         <v>0.96069868995633101</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -4931,16 +7084,39 @@
         <v>8</v>
       </c>
       <c r="C33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" t="s">
         <v>14</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>15</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>17</v>
       </c>
+      <c r="P33" t="str">
+        <f>A33</f>
+        <v>Simulation</v>
+      </c>
+      <c r="Q33" t="str">
+        <f t="shared" ref="Q33:T48" si="3">B33</f>
+        <v>Date</v>
+      </c>
+      <c r="R33" t="str">
+        <f t="shared" si="3"/>
+        <v>Gliricidia.AboveGround.Wt</v>
+      </c>
+      <c r="S33" t="str">
+        <f t="shared" si="3"/>
+        <v>Gliricidia.Leaf.Live.Wt</v>
+      </c>
+      <c r="T33" t="str">
+        <f t="shared" si="3"/>
+        <v>Gliricidia.Stem.Live.Wt</v>
+      </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -4948,145 +7124,289 @@
         <f>B9</f>
         <v>35184.124463519314</v>
       </c>
-      <c r="C34">
-        <f>D9*$E$5*1000</f>
+      <c r="C34" s="4">
+        <f>D34+E34</f>
+        <v>382.14438342985062</v>
+      </c>
+      <c r="D34">
+        <f>E9*$F$5*1000</f>
         <v>272.10071530758057</v>
       </c>
-      <c r="D34">
-        <f>E9*$E$5*1000</f>
+      <c r="E34">
+        <f>F9*$F$5*1000</f>
         <v>110.04366812227003</v>
       </c>
-      <c r="E34">
-        <f>D15*$E$5*1000</f>
+      <c r="F34">
+        <f>E15*$F$5*1000</f>
         <v>0</v>
       </c>
+      <c r="P34" t="str">
+        <f t="shared" ref="P34:P56" si="4">A34</f>
+        <v>GuadeloupeHarvest12Month</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="3"/>
+        <v>35184.124463519314</v>
+      </c>
+      <c r="R34">
+        <f t="shared" si="3"/>
+        <v>382.14438342985062</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="3"/>
+        <v>272.10071530758057</v>
+      </c>
+      <c r="T34">
+        <f t="shared" si="3"/>
+        <v>110.04366812227003</v>
+      </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>10</v>
       </c>
       <c r="B35" s="2">
-        <f t="shared" ref="B35:B39" si="3">B10</f>
+        <f t="shared" ref="B35:B39" si="5">B10</f>
         <v>35236.038626609443</v>
       </c>
-      <c r="C35">
-        <f t="shared" ref="C35:D39" si="4">D10*$E$5*1000</f>
+      <c r="C35" s="4">
+        <f t="shared" ref="C35:C56" si="6">D35+E35</f>
+        <v>1751.4978428322415</v>
+      </c>
+      <c r="D35">
+        <f t="shared" ref="D35:E39" si="7">E10*$F$5*1000</f>
         <v>871.14849785407705</v>
       </c>
-      <c r="D35">
+      <c r="E35">
+        <f t="shared" si="7"/>
+        <v>880.34934497816437</v>
+      </c>
+      <c r="F35">
+        <f t="shared" ref="F35:F39" si="8">E16*$F$5*1000</f>
+        <v>47.948497854077509</v>
+      </c>
+      <c r="P35" t="str">
         <f t="shared" si="4"/>
+        <v>GuadeloupeHarvest12Month</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="3"/>
+        <v>35236.038626609443</v>
+      </c>
+      <c r="R35">
+        <f t="shared" si="3"/>
+        <v>1751.4978428322415</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="3"/>
+        <v>871.14849785407705</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="3"/>
         <v>880.34934497816437</v>
       </c>
-      <c r="E35">
-        <f t="shared" ref="E35:E39" si="5">D16*$E$5*1000</f>
-        <v>47.948497854077509</v>
-      </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>10</v>
       </c>
       <c r="B36" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>35290.836909871243</v>
       </c>
-      <c r="C36">
-        <f>D11*$E$5*1000</f>
+      <c r="C36" s="4">
+        <f t="shared" si="6"/>
+        <v>4171.4279338543429</v>
+      </c>
+      <c r="D36">
+        <f>E11*$F$5*1000</f>
         <v>1457.0174535050062</v>
       </c>
-      <c r="D36">
-        <f t="shared" si="4"/>
+      <c r="E36">
+        <f t="shared" si="7"/>
         <v>2714.4104803493365</v>
       </c>
-      <c r="E36">
-        <f t="shared" si="5"/>
+      <c r="F36">
+        <f t="shared" si="8"/>
         <v>333.34020028612167</v>
       </c>
-      <c r="I36" s="2"/>
-      <c r="J36" s="3"/>
+      <c r="J36" s="2"/>
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+      <c r="P36" t="str">
+        <f t="shared" si="4"/>
+        <v>GuadeloupeHarvest12Month</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="3"/>
+        <v>35290.836909871243</v>
+      </c>
+      <c r="R36">
+        <f t="shared" si="3"/>
+        <v>4171.4279338543429</v>
+      </c>
+      <c r="S36">
+        <f t="shared" si="3"/>
+        <v>1457.0174535050062</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="3"/>
+        <v>2714.4104803493365</v>
+      </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>10</v>
       </c>
       <c r="B37" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>35348.519313304721</v>
       </c>
-      <c r="C37">
-        <f t="shared" si="4"/>
+      <c r="C37" s="4">
+        <f t="shared" si="6"/>
+        <v>5409.7355298586226</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="7"/>
         <v>971.30758226037051</v>
       </c>
-      <c r="D37">
-        <f t="shared" si="4"/>
+      <c r="E37">
+        <f t="shared" si="7"/>
         <v>4438.4279475982521</v>
       </c>
-      <c r="E37">
-        <f t="shared" si="5"/>
+      <c r="F37">
+        <f t="shared" si="8"/>
         <v>500.90758226037059</v>
       </c>
-      <c r="I37" s="2"/>
-      <c r="J37" s="3"/>
+      <c r="J37" s="2"/>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="P37" t="str">
+        <f t="shared" si="4"/>
+        <v>GuadeloupeHarvest12Month</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="3"/>
+        <v>35348.519313304721</v>
+      </c>
+      <c r="R37">
+        <f t="shared" si="3"/>
+        <v>5409.7355298586226</v>
+      </c>
+      <c r="S37">
+        <f t="shared" si="3"/>
+        <v>971.30758226037051</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="3"/>
+        <v>4438.4279475982521</v>
+      </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>10</v>
       </c>
       <c r="B38" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>35400.43347639485</v>
       </c>
-      <c r="C38">
-        <f t="shared" si="4"/>
+      <c r="C38" s="4">
+        <f t="shared" si="6"/>
+        <v>7011.6153356947761</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="7"/>
         <v>812.48869814020009</v>
       </c>
-      <c r="D38">
-        <f t="shared" si="4"/>
+      <c r="E38">
+        <f t="shared" si="7"/>
         <v>6199.1266375545765</v>
       </c>
-      <c r="E38">
-        <f t="shared" si="5"/>
+      <c r="F38">
+        <f t="shared" si="8"/>
         <v>289.82203147353323</v>
       </c>
-      <c r="I38" s="2"/>
-      <c r="J38" s="3"/>
+      <c r="J38" s="2"/>
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+      <c r="P38" t="str">
+        <f t="shared" si="4"/>
+        <v>GuadeloupeHarvest12Month</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" si="3"/>
+        <v>35400.43347639485</v>
+      </c>
+      <c r="R38">
+        <f t="shared" si="3"/>
+        <v>7011.6153356947761</v>
+      </c>
+      <c r="S38">
+        <f t="shared" si="3"/>
+        <v>812.48869814020009</v>
+      </c>
+      <c r="T38">
+        <f t="shared" si="3"/>
+        <v>6199.1266375545765</v>
+      </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>10</v>
       </c>
       <c r="B39" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>35461</v>
       </c>
-      <c r="C39">
-        <f t="shared" si="4"/>
+      <c r="C39" s="4">
+        <f t="shared" si="6"/>
+        <v>4909.3007278020277</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="7"/>
         <v>287.46666666666687</v>
       </c>
-      <c r="D39">
-        <f t="shared" si="4"/>
+      <c r="E39">
+        <f t="shared" si="7"/>
         <v>4621.8340611353606</v>
       </c>
-      <c r="E39">
-        <f t="shared" si="5"/>
+      <c r="F39">
+        <f t="shared" si="8"/>
         <v>182.93333333333328</v>
       </c>
-      <c r="I39" s="2"/>
-      <c r="J39" s="3"/>
+      <c r="J39" s="2"/>
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="P39" t="str">
+        <f t="shared" si="4"/>
+        <v>GuadeloupeHarvest12Month</v>
+      </c>
+      <c r="Q39">
+        <f t="shared" si="3"/>
+        <v>35461</v>
+      </c>
+      <c r="R39">
+        <f t="shared" si="3"/>
+        <v>4909.3007278020277</v>
+      </c>
+      <c r="S39">
+        <f t="shared" si="3"/>
+        <v>287.46666666666687</v>
+      </c>
+      <c r="T39">
+        <f t="shared" si="3"/>
+        <v>4621.8340611353606</v>
+      </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>16</v>
       </c>
@@ -5094,77 +7414,149 @@
         <f>B34</f>
         <v>35184.124463519314</v>
       </c>
-      <c r="C40">
-        <f>I9*$E$5*1000</f>
+      <c r="C40" s="4">
+        <f t="shared" si="6"/>
+        <v>272.12268646760583</v>
+      </c>
+      <c r="D40">
+        <f>J9*$F$5*1000</f>
         <v>195.6612399643173</v>
       </c>
-      <c r="D40">
-        <f>J9*$E$5*1000</f>
+      <c r="E40">
+        <f>K9*$F$5*1000</f>
         <v>76.461446503288556</v>
       </c>
-      <c r="E40">
-        <f>I15*$E$5*1000</f>
+      <c r="F40">
+        <f>J15*$F$5*1000</f>
         <v>0</v>
       </c>
-      <c r="I40" s="2"/>
-      <c r="J40" s="3"/>
+      <c r="J40" s="2"/>
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
+      <c r="P40" t="str">
+        <f t="shared" si="4"/>
+        <v>GuadeloupeHarvest06Month</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" si="3"/>
+        <v>35184.124463519314</v>
+      </c>
+      <c r="R40">
+        <f t="shared" si="3"/>
+        <v>272.12268646760583</v>
+      </c>
+      <c r="S40">
+        <f t="shared" si="3"/>
+        <v>195.6612399643173</v>
+      </c>
+      <c r="T40">
+        <f t="shared" si="3"/>
+        <v>76.461446503288556</v>
+      </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>16</v>
       </c>
       <c r="B41" s="2">
-        <f t="shared" ref="B41:B42" si="6">B35</f>
+        <f t="shared" ref="B41:B42" si="9">B35</f>
         <v>35236.038626609443</v>
       </c>
-      <c r="C41">
-        <f t="shared" ref="C41:D41" si="7">I10*$E$5*1000</f>
+      <c r="C41" s="4">
+        <f t="shared" si="6"/>
+        <v>1466.848726400782</v>
+      </c>
+      <c r="D41">
+        <f t="shared" ref="D41:E41" si="10">J10*$F$5*1000</f>
         <v>752.15655664585154</v>
       </c>
-      <c r="D41">
-        <f t="shared" si="7"/>
+      <c r="E41">
+        <f t="shared" si="10"/>
         <v>714.69216975493043</v>
       </c>
-      <c r="E41">
-        <f t="shared" ref="E41:E42" si="8">I16*$E$5*1000</f>
+      <c r="F41">
+        <f t="shared" ref="F41:F42" si="11">J16*$F$5*1000</f>
         <v>30.051293487956993</v>
       </c>
-      <c r="I41" s="2"/>
-      <c r="J41" s="3"/>
+      <c r="J41" s="2"/>
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
+      <c r="P41" t="str">
+        <f t="shared" si="4"/>
+        <v>GuadeloupeHarvest06Month</v>
+      </c>
+      <c r="Q41">
+        <f t="shared" si="3"/>
+        <v>35236.038626609443</v>
+      </c>
+      <c r="R41">
+        <f t="shared" si="3"/>
+        <v>1466.848726400782</v>
+      </c>
+      <c r="S41">
+        <f t="shared" si="3"/>
+        <v>752.15655664585154</v>
+      </c>
+      <c r="T41">
+        <f t="shared" si="3"/>
+        <v>714.69216975493043</v>
+      </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>16</v>
       </c>
       <c r="B42" s="2">
+        <f t="shared" si="9"/>
+        <v>35290.836909871243</v>
+      </c>
+      <c r="C42" s="4">
         <f t="shared" si="6"/>
-        <v>35290.836909871243</v>
-      </c>
-      <c r="C42">
-        <f t="shared" ref="C42:D42" si="9">I11*$E$5*1000</f>
+        <v>3619.9403497752191</v>
+      </c>
+      <c r="D42">
+        <f t="shared" ref="D42:E42" si="12">J11*$F$5*1000</f>
         <v>1282.9170383586077</v>
       </c>
-      <c r="D42">
-        <f t="shared" si="9"/>
+      <c r="E42">
+        <f t="shared" si="12"/>
         <v>2337.0233114166117</v>
       </c>
-      <c r="E42">
-        <f t="shared" si="8"/>
+      <c r="F42">
+        <f t="shared" si="11"/>
         <v>290.02230151650213</v>
       </c>
-      <c r="I42" s="2"/>
-      <c r="J42" s="3"/>
+      <c r="J42" s="2"/>
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
+      <c r="N42" s="3"/>
+      <c r="P42" t="str">
+        <f t="shared" si="4"/>
+        <v>GuadeloupeHarvest06Month</v>
+      </c>
+      <c r="Q42">
+        <f t="shared" si="3"/>
+        <v>35290.836909871243</v>
+      </c>
+      <c r="R42">
+        <f t="shared" si="3"/>
+        <v>3619.9403497752191</v>
+      </c>
+      <c r="S42">
+        <f t="shared" si="3"/>
+        <v>1282.9170383586077</v>
+      </c>
+      <c r="T42">
+        <f t="shared" si="3"/>
+        <v>2337.0233114166117</v>
+      </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -5172,19 +7564,43 @@
         <f>B42</f>
         <v>35290.836909871243</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="4">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D43">
         <v>0</v>
       </c>
-      <c r="I43" s="2"/>
-      <c r="J43" s="3"/>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="J43" s="2"/>
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
+      <c r="P43" t="str">
+        <f t="shared" si="4"/>
+        <v>GuadeloupeHarvest06Month</v>
+      </c>
+      <c r="Q43">
+        <f t="shared" si="3"/>
+        <v>35290.836909871243</v>
+      </c>
+      <c r="R43">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S43">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T43">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>16</v>
       </c>
@@ -5192,20 +7608,44 @@
         <f>B37</f>
         <v>35348.519313304721</v>
       </c>
-      <c r="C44">
-        <f t="shared" ref="C44:D44" si="10">I12*$E$5*1000</f>
+      <c r="C44" s="4">
+        <f t="shared" si="6"/>
+        <v>729.44577132320444</v>
+      </c>
+      <c r="D44">
+        <f t="shared" ref="D44:E44" si="13">J12*$F$5*1000</f>
         <v>459.89406779660811</v>
       </c>
-      <c r="D44">
-        <f t="shared" si="10"/>
+      <c r="E44">
+        <f t="shared" si="13"/>
         <v>269.55170352659633</v>
       </c>
-      <c r="E44">
-        <f>I18*$E$5*1000</f>
+      <c r="F44">
+        <f>J18*$F$5*1000</f>
         <v>21.473015165030727</v>
       </c>
+      <c r="P44" t="str">
+        <f t="shared" si="4"/>
+        <v>GuadeloupeHarvest06Month</v>
+      </c>
+      <c r="Q44">
+        <f t="shared" si="3"/>
+        <v>35348.519313304721</v>
+      </c>
+      <c r="R44">
+        <f t="shared" si="3"/>
+        <v>729.44577132320444</v>
+      </c>
+      <c r="S44">
+        <f t="shared" si="3"/>
+        <v>459.89406779660811</v>
+      </c>
+      <c r="T44">
+        <f t="shared" si="3"/>
+        <v>269.55170352659633</v>
+      </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>16</v>
       </c>
@@ -5213,20 +7653,44 @@
         <f>B38</f>
         <v>35400.43347639485</v>
       </c>
-      <c r="C45">
-        <f t="shared" ref="C45:D45" si="11">I13*$E$5*1000</f>
+      <c r="C45" s="4">
+        <f t="shared" si="6"/>
+        <v>1376.630206197714</v>
+      </c>
+      <c r="D45">
+        <f t="shared" ref="D45:E45" si="14">J13*$F$5*1000</f>
         <v>539.28412132024903</v>
       </c>
-      <c r="D45">
-        <f t="shared" si="11"/>
+      <c r="E45">
+        <f t="shared" si="14"/>
         <v>837.34608487746493</v>
       </c>
-      <c r="E45">
-        <f>I19*$E$5*1000</f>
+      <c r="F45">
+        <f>J19*$F$5*1000</f>
         <v>191.12622658340734</v>
       </c>
+      <c r="P45" t="str">
+        <f t="shared" si="4"/>
+        <v>GuadeloupeHarvest06Month</v>
+      </c>
+      <c r="Q45">
+        <f t="shared" si="3"/>
+        <v>35400.43347639485</v>
+      </c>
+      <c r="R45">
+        <f t="shared" si="3"/>
+        <v>1376.630206197714</v>
+      </c>
+      <c r="S45">
+        <f t="shared" si="3"/>
+        <v>539.28412132024903</v>
+      </c>
+      <c r="T45">
+        <f t="shared" si="3"/>
+        <v>837.34608487746493</v>
+      </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>16</v>
       </c>
@@ -5234,20 +7698,44 @@
         <f>B39</f>
         <v>35461</v>
       </c>
-      <c r="C46">
-        <f>I14*$E$5*1000</f>
+      <c r="C46" s="4">
+        <f t="shared" si="6"/>
+        <v>1427.1389813712315</v>
+      </c>
+      <c r="D46">
+        <f>J14*$F$5*1000</f>
         <v>232.15990187332525</v>
       </c>
-      <c r="D46">
-        <f>J14*$E$5*1000</f>
+      <c r="E46">
+        <f>K14*$F$5*1000</f>
         <v>1194.9790794979062</v>
       </c>
-      <c r="E46">
-        <f>I20*$E$5*1000</f>
+      <c r="F46">
+        <f>J20*$F$5*1000</f>
         <v>296.57894736841979</v>
       </c>
+      <c r="P46" t="str">
+        <f t="shared" si="4"/>
+        <v>GuadeloupeHarvest06Month</v>
+      </c>
+      <c r="Q46">
+        <f t="shared" si="3"/>
+        <v>35461</v>
+      </c>
+      <c r="R46">
+        <f t="shared" si="3"/>
+        <v>1427.1389813712315</v>
+      </c>
+      <c r="S46">
+        <f t="shared" si="3"/>
+        <v>232.15990187332525</v>
+      </c>
+      <c r="T46">
+        <f t="shared" si="3"/>
+        <v>1194.9790794979062</v>
+      </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>18</v>
       </c>
@@ -5255,20 +7743,44 @@
         <f>B40</f>
         <v>35184.124463519314</v>
       </c>
-      <c r="C47">
-        <f t="shared" ref="C47:C56" si="12">O9*$E$5*1000</f>
+      <c r="C47" s="4">
+        <f t="shared" si="6"/>
         <v>53.091847192281655</v>
       </c>
       <c r="D47">
-        <f t="shared" ref="D47:D56" si="13">Q9*$E$5*1000</f>
+        <f t="shared" ref="D47:D56" si="15">P9*$F$5*1000</f>
+        <v>53.091847192281655</v>
+      </c>
+      <c r="E47">
+        <f t="shared" ref="E47:E56" si="16">R9*$F$5*1000</f>
         <v>0</v>
       </c>
-      <c r="E47">
-        <f>O19*$E$5*1000</f>
+      <c r="F47">
+        <f>P19*$F$5*1000</f>
         <v>0</v>
       </c>
+      <c r="P47" t="str">
+        <f t="shared" si="4"/>
+        <v>GuadeloupeHarvest02Month</v>
+      </c>
+      <c r="Q47">
+        <f t="shared" si="3"/>
+        <v>35184.124463519314</v>
+      </c>
+      <c r="R47">
+        <f t="shared" si="3"/>
+        <v>53.091847192281655</v>
+      </c>
+      <c r="S47">
+        <f t="shared" si="3"/>
+        <v>53.091847192281655</v>
+      </c>
+      <c r="T47">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>18</v>
       </c>
@@ -5276,20 +7788,44 @@
         <f>B41</f>
         <v>35236.038626609443</v>
       </c>
-      <c r="C48">
-        <f t="shared" si="12"/>
+      <c r="C48" s="4">
+        <f t="shared" si="6"/>
+        <v>789.47429580773655</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="15"/>
         <v>385.9808460260781</v>
       </c>
-      <c r="D48">
-        <f t="shared" si="13"/>
+      <c r="E48">
+        <f t="shared" si="16"/>
         <v>403.49344978165851</v>
       </c>
-      <c r="E48">
-        <f>O20*$E$5*1000</f>
+      <c r="F48">
+        <f>P20*$F$5*1000</f>
         <v>29.610912817612764</v>
       </c>
+      <c r="P48" t="str">
+        <f t="shared" si="4"/>
+        <v>GuadeloupeHarvest02Month</v>
+      </c>
+      <c r="Q48">
+        <f t="shared" si="3"/>
+        <v>35236.038626609443</v>
+      </c>
+      <c r="R48">
+        <f t="shared" si="3"/>
+        <v>789.47429580773655</v>
+      </c>
+      <c r="S48">
+        <f t="shared" si="3"/>
+        <v>385.9808460260781</v>
+      </c>
+      <c r="T48">
+        <f t="shared" si="3"/>
+        <v>403.49344978165851</v>
+      </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>18</v>
       </c>
@@ -5297,16 +7833,40 @@
         <f>B48</f>
         <v>35236.038626609443</v>
       </c>
-      <c r="C49">
-        <f t="shared" si="12"/>
+      <c r="C49" s="4">
+        <f t="shared" si="6"/>
+        <v>329.06577502236286</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="15"/>
         <v>182.34088419267016</v>
       </c>
-      <c r="D49">
-        <f t="shared" si="13"/>
+      <c r="E49">
+        <f t="shared" si="16"/>
         <v>146.7248908296927</v>
       </c>
+      <c r="P49" t="str">
+        <f t="shared" si="4"/>
+        <v>GuadeloupeHarvest02Month</v>
+      </c>
+      <c r="Q49">
+        <f t="shared" ref="Q49:Q56" si="17">B49</f>
+        <v>35236.038626609443</v>
+      </c>
+      <c r="R49">
+        <f t="shared" ref="R49:R56" si="18">C49</f>
+        <v>329.06577502236286</v>
+      </c>
+      <c r="S49">
+        <f t="shared" ref="S49:S56" si="19">D49</f>
+        <v>182.34088419267016</v>
+      </c>
+      <c r="T49">
+        <f t="shared" ref="T49:T56" si="20">E49</f>
+        <v>146.7248908296927</v>
+      </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
         <v>18</v>
       </c>
@@ -5314,20 +7874,44 @@
         <f>B42</f>
         <v>35290.836909871243</v>
       </c>
-      <c r="C50">
-        <f t="shared" si="12"/>
+      <c r="C50" s="4">
+        <f t="shared" si="6"/>
+        <v>1059.4950920623123</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="15"/>
         <v>362.55186062126631</v>
       </c>
-      <c r="D50">
-        <f t="shared" si="13"/>
+      <c r="E50">
+        <f t="shared" si="16"/>
         <v>696.94323144104601</v>
       </c>
-      <c r="E50">
-        <f>O21*$E$5*1000</f>
+      <c r="F50">
+        <f>P21*$F$5*1000</f>
         <v>108.10580626921592</v>
       </c>
+      <c r="P50" t="str">
+        <f t="shared" si="4"/>
+        <v>GuadeloupeHarvest02Month</v>
+      </c>
+      <c r="Q50">
+        <f t="shared" si="17"/>
+        <v>35290.836909871243</v>
+      </c>
+      <c r="R50">
+        <f t="shared" si="18"/>
+        <v>1059.4950920623123</v>
+      </c>
+      <c r="S50">
+        <f t="shared" si="19"/>
+        <v>362.55186062126631</v>
+      </c>
+      <c r="T50">
+        <f t="shared" si="20"/>
+        <v>696.94323144104601</v>
+      </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
         <v>18</v>
       </c>
@@ -5335,16 +7919,40 @@
         <f>B50</f>
         <v>35290.836909871243</v>
       </c>
-      <c r="C51">
-        <f t="shared" si="12"/>
+      <c r="C51" s="4">
+        <f t="shared" si="6"/>
+        <v>465.19307600154139</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="15"/>
         <v>171.74329434215599</v>
       </c>
-      <c r="D51">
-        <f t="shared" si="13"/>
+      <c r="E51">
+        <f t="shared" si="16"/>
         <v>293.44978165938539</v>
       </c>
+      <c r="P51" t="str">
+        <f t="shared" si="4"/>
+        <v>GuadeloupeHarvest02Month</v>
+      </c>
+      <c r="Q51">
+        <f t="shared" si="17"/>
+        <v>35290.836909871243</v>
+      </c>
+      <c r="R51">
+        <f t="shared" si="18"/>
+        <v>465.19307600154139</v>
+      </c>
+      <c r="S51">
+        <f t="shared" si="19"/>
+        <v>171.74329434215599</v>
+      </c>
+      <c r="T51">
+        <f t="shared" si="20"/>
+        <v>293.44978165938539</v>
+      </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
         <v>18</v>
       </c>
@@ -5352,20 +7960,44 @@
         <f>B44</f>
         <v>35348.519313304721</v>
       </c>
-      <c r="C52">
-        <f t="shared" si="12"/>
+      <c r="C52" s="4">
+        <f t="shared" si="6"/>
+        <v>934.50587059007205</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="15"/>
         <v>237.56263914902607</v>
       </c>
-      <c r="D52">
-        <f t="shared" si="13"/>
+      <c r="E52">
+        <f t="shared" si="16"/>
         <v>696.94323144104601</v>
       </c>
-      <c r="E52">
-        <f>O22*$E$5*1000</f>
+      <c r="F52">
+        <f>P22*$F$5*1000</f>
         <v>84.832667773968865</v>
       </c>
+      <c r="P52" t="str">
+        <f t="shared" si="4"/>
+        <v>GuadeloupeHarvest02Month</v>
+      </c>
+      <c r="Q52">
+        <f t="shared" si="17"/>
+        <v>35348.519313304721</v>
+      </c>
+      <c r="R52">
+        <f t="shared" si="18"/>
+        <v>934.50587059007205</v>
+      </c>
+      <c r="S52">
+        <f t="shared" si="19"/>
+        <v>237.56263914902607</v>
+      </c>
+      <c r="T52">
+        <f t="shared" si="20"/>
+        <v>696.94323144104601</v>
+      </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
         <v>18</v>
       </c>
@@ -5373,16 +8005,40 @@
         <f>B52</f>
         <v>35348.519313304721</v>
       </c>
-      <c r="C53">
-        <f t="shared" si="12"/>
+      <c r="C53" s="4">
+        <f t="shared" si="6"/>
+        <v>193.37506575989741</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="15"/>
         <v>46.650174930204713</v>
       </c>
-      <c r="D53">
-        <f t="shared" si="13"/>
+      <c r="E53">
+        <f t="shared" si="16"/>
         <v>146.7248908296927</v>
       </c>
+      <c r="P53" t="str">
+        <f t="shared" si="4"/>
+        <v>GuadeloupeHarvest02Month</v>
+      </c>
+      <c r="Q53">
+        <f t="shared" si="17"/>
+        <v>35348.519313304721</v>
+      </c>
+      <c r="R53">
+        <f t="shared" si="18"/>
+        <v>193.37506575989741</v>
+      </c>
+      <c r="S53">
+        <f t="shared" si="19"/>
+        <v>46.650174930204713</v>
+      </c>
+      <c r="T53">
+        <f t="shared" si="20"/>
+        <v>146.7248908296927</v>
+      </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
         <v>18</v>
       </c>
@@ -5390,20 +8046,44 @@
         <f>B45</f>
         <v>35400.43347639485</v>
       </c>
-      <c r="C54">
-        <f t="shared" si="12"/>
+      <c r="C54" s="4">
+        <f t="shared" si="6"/>
+        <v>1107.1065983972544</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="15"/>
         <v>226.75725341909006</v>
       </c>
-      <c r="D54">
-        <f t="shared" si="13"/>
+      <c r="E54">
+        <f t="shared" si="16"/>
         <v>880.34934497816437</v>
       </c>
-      <c r="E54">
-        <f>O23*$E$5*1000</f>
+      <c r="F54">
+        <f>P23*$F$5*1000</f>
         <v>61.351733399300393</v>
       </c>
+      <c r="P54" t="str">
+        <f t="shared" si="4"/>
+        <v>GuadeloupeHarvest02Month</v>
+      </c>
+      <c r="Q54">
+        <f t="shared" si="17"/>
+        <v>35400.43347639485</v>
+      </c>
+      <c r="R54">
+        <f t="shared" si="18"/>
+        <v>1107.1065983972544</v>
+      </c>
+      <c r="S54">
+        <f t="shared" si="19"/>
+        <v>226.75725341909006</v>
+      </c>
+      <c r="T54">
+        <f t="shared" si="20"/>
+        <v>880.34934497816437</v>
+      </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
         <v>18</v>
       </c>
@@ -5411,16 +8091,40 @@
         <f>B54</f>
         <v>35400.43347639485</v>
       </c>
-      <c r="C55">
-        <f t="shared" si="12"/>
+      <c r="C55" s="4">
+        <f t="shared" si="6"/>
+        <v>416.88578402543004</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="15"/>
         <v>86.754779658621047</v>
       </c>
-      <c r="D55">
-        <f t="shared" si="13"/>
+      <c r="E55">
+        <f t="shared" si="16"/>
         <v>330.13100436680901</v>
       </c>
+      <c r="P55" t="str">
+        <f t="shared" si="4"/>
+        <v>GuadeloupeHarvest02Month</v>
+      </c>
+      <c r="Q55">
+        <f t="shared" si="17"/>
+        <v>35400.43347639485</v>
+      </c>
+      <c r="R55">
+        <f t="shared" si="18"/>
+        <v>416.88578402543004</v>
+      </c>
+      <c r="S55">
+        <f t="shared" si="19"/>
+        <v>86.754779658621047</v>
+      </c>
+      <c r="T55">
+        <f t="shared" si="20"/>
+        <v>330.13100436680901</v>
+      </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
         <v>18</v>
       </c>
@@ -5428,21 +8132,46 @@
         <f>B46</f>
         <v>35461</v>
       </c>
-      <c r="C56">
-        <f t="shared" si="12"/>
+      <c r="C56" s="4">
+        <f t="shared" si="6"/>
+        <v>248.49292277654183</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="15"/>
         <v>101.76803194684915</v>
       </c>
-      <c r="D56">
-        <f t="shared" si="13"/>
+      <c r="E56">
+        <f t="shared" si="16"/>
         <v>146.7248908296927</v>
       </c>
-      <c r="E56">
-        <f>O24*$E$5*1000</f>
+      <c r="F56">
+        <f>P24*$F$5*1000</f>
         <v>127.22302717602533</v>
       </c>
+      <c r="P56" t="str">
+        <f t="shared" si="4"/>
+        <v>GuadeloupeHarvest02Month</v>
+      </c>
+      <c r="Q56">
+        <f t="shared" si="17"/>
+        <v>35461</v>
+      </c>
+      <c r="R56">
+        <f t="shared" si="18"/>
+        <v>248.49292277654183</v>
+      </c>
+      <c r="S56">
+        <f t="shared" si="19"/>
+        <v>101.76803194684915</v>
+      </c>
+      <c r="T56">
+        <f t="shared" si="20"/>
+        <v>146.7248908296927</v>
+      </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>